<commit_message>
:package: funtion to criate tab_log created
</commit_message>
<xml_diff>
--- a/logs/testes_lk_fuzzy.xlsx
+++ b/logs/testes_lk_fuzzy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\files\projects\programacao\python\acoes_data\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A64CD3A-DA98-438A-827E-BC6D57F9BDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C33C9E-BB19-4E81-98B0-13695592BFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>data e hora</t>
   </si>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,6 +862,93 @@
         <v>3</v>
       </c>
     </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45240.451724537037</v>
+      </c>
+      <c r="B17">
+        <v>0.189500560923064</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>0.2</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45240.458680555559</v>
+      </c>
+      <c r="B18">
+        <v>0.18807162723138701</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>0.2</v>
+      </c>
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45240.468680555554</v>
+      </c>
+      <c r="B19">
+        <v>0.19220388202041699</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>0.2</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>